<commit_message>
replaced buttons with dropdown, some bugfixes and minor layout changes
</commit_message>
<xml_diff>
--- a/collection.xlsx
+++ b/collection.xlsx
@@ -854,9 +854,6 @@
     <t>BeyBlade: Super Tournament Battle</t>
   </si>
   <si>
-    <t>1080° Avalanche</t>
-  </si>
-  <si>
     <t>XIII</t>
   </si>
   <si>
@@ -1665,6 +1662,9 @@
   </si>
   <si>
     <t>http://i238.photobucket.com/albums/ff172/benjamin_fun/Games/20170606_214139_zpsjolyfga8.jpg</t>
+  </si>
+  <si>
+    <t>1080 Avalanche</t>
   </si>
 </sst>
 </file>
@@ -2013,8 +2013,8 @@
   <dimension ref="A1:P1144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,22 +2056,22 @@
         <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L1" t="s">
+        <v>531</v>
+      </c>
+      <c r="M1" t="s">
         <v>532</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>533</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>534</v>
       </c>
-      <c r="O1" t="s">
-        <v>535</v>
-      </c>
       <c r="P1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2135,16 +2135,16 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
+        <v>544</v>
+      </c>
+      <c r="L3" t="s">
         <v>545</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>546</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>547</v>
-      </c>
-      <c r="N3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2253,19 +2253,19 @@
         <v>10</v>
       </c>
       <c r="K8" t="s">
+        <v>526</v>
+      </c>
+      <c r="L8" t="s">
         <v>527</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" t="s">
         <v>529</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>530</v>
-      </c>
-      <c r="O8" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
         <v>37305</v>
       </c>
       <c r="G9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>37324</v>
       </c>
       <c r="G10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2401,16 +2401,16 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
+        <v>540</v>
+      </c>
+      <c r="L13" t="s">
         <v>541</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>542</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>543</v>
-      </c>
-      <c r="N13" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3881,7 +3881,7 @@
         <v>37538</v>
       </c>
       <c r="G66" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -7521,7 +7521,7 @@
         <v>37928</v>
       </c>
       <c r="G221" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -7717,7 +7717,7 @@
         <v>37943</v>
       </c>
       <c r="G229" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7837,7 +7837,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>278</v>
+        <v>548</v>
       </c>
       <c r="B235" t="s">
         <v>9</v>
@@ -7860,7 +7860,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B236" t="s">
         <v>9</v>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B237" t="s">
         <v>9</v>
@@ -7906,7 +7906,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B238" t="s">
         <v>9</v>
@@ -7929,7 +7929,7 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B239" t="s">
         <v>9</v>
@@ -7952,7 +7952,7 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B240" t="s">
         <v>9</v>
@@ -7975,7 +7975,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B241" t="s">
         <v>9</v>
@@ -7998,7 +7998,7 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B242" t="s">
         <v>9</v>
@@ -8021,7 +8021,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B243" t="s">
         <v>9</v>
@@ -8039,12 +8039,12 @@
         <v>37959</v>
       </c>
       <c r="G243" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B244" t="s">
         <v>9</v>
@@ -8073,7 +8073,7 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B245" t="s">
         <v>9</v>
@@ -8096,7 +8096,7 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B246" t="s">
         <v>9</v>
@@ -8119,7 +8119,7 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B247" t="s">
         <v>9</v>
@@ -8148,7 +8148,7 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B248" t="s">
         <v>9</v>
@@ -8177,7 +8177,7 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B249" t="s">
         <v>9</v>
@@ -8200,7 +8200,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B250" t="s">
         <v>9</v>
@@ -8223,7 +8223,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B251" t="s">
         <v>9</v>
@@ -8246,7 +8246,7 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B252" t="s">
         <v>9</v>
@@ -8269,7 +8269,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B253" t="s">
         <v>9</v>
@@ -8292,7 +8292,7 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B254" t="s">
         <v>9</v>
@@ -8315,7 +8315,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B255" t="s">
         <v>9</v>
@@ -8338,7 +8338,7 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B256" t="s">
         <v>9</v>
@@ -8361,7 +8361,7 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B257" t="s">
         <v>9</v>
@@ -8384,7 +8384,7 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B258" t="s">
         <v>9</v>
@@ -8407,7 +8407,7 @@
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B259" t="s">
         <v>9</v>
@@ -8430,7 +8430,7 @@
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B260" t="s">
         <v>9</v>
@@ -8459,7 +8459,7 @@
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B261" t="s">
         <v>9</v>
@@ -8482,7 +8482,7 @@
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B262" t="s">
         <v>9</v>
@@ -8505,7 +8505,7 @@
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B263" t="s">
         <v>9</v>
@@ -8528,7 +8528,7 @@
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B264" t="s">
         <v>9</v>
@@ -8551,7 +8551,7 @@
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B265" t="s">
         <v>9</v>
@@ -8574,7 +8574,7 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B266" t="s">
         <v>9</v>
@@ -8597,7 +8597,7 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B267" t="s">
         <v>9</v>
@@ -8620,7 +8620,7 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B268" t="s">
         <v>9</v>
@@ -8643,7 +8643,7 @@
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B269" t="s">
         <v>9</v>
@@ -8664,12 +8664,12 @@
         <v>52</v>
       </c>
       <c r="P269" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B270" t="s">
         <v>9</v>
@@ -8692,7 +8692,7 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B271" t="s">
         <v>9</v>
@@ -8715,7 +8715,7 @@
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B272" t="s">
         <v>9</v>
@@ -8738,7 +8738,7 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B273" t="s">
         <v>9</v>
@@ -8761,7 +8761,7 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B274" t="s">
         <v>9</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B275" t="s">
         <v>9</v>
@@ -8807,7 +8807,7 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B276" t="s">
         <v>9</v>
@@ -8830,7 +8830,7 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B277" t="s">
         <v>9</v>
@@ -8853,7 +8853,7 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B278" t="s">
         <v>9</v>
@@ -8876,7 +8876,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B279" t="s">
         <v>9</v>
@@ -8899,7 +8899,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B280" t="s">
         <v>9</v>
@@ -8928,7 +8928,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B281" t="s">
         <v>9</v>
@@ -8951,7 +8951,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B282" t="s">
         <v>9</v>
@@ -8974,7 +8974,7 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B283" t="s">
         <v>9</v>
@@ -9003,7 +9003,7 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B284" t="s">
         <v>9</v>
@@ -9026,7 +9026,7 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B285" t="s">
         <v>9</v>
@@ -9049,7 +9049,7 @@
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B286" t="s">
         <v>9</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B287" t="s">
         <v>9</v>
@@ -9090,12 +9090,12 @@
         <v>38096</v>
       </c>
       <c r="G287" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B288" t="s">
         <v>9</v>
@@ -9118,7 +9118,7 @@
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B289" t="s">
         <v>9</v>
@@ -9141,7 +9141,7 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B290" t="s">
         <v>9</v>
@@ -9168,12 +9168,12 @@
         <v>12</v>
       </c>
       <c r="P290" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B291" t="s">
         <v>9</v>
@@ -9202,7 +9202,7 @@
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B292" t="s">
         <v>9</v>
@@ -9231,7 +9231,7 @@
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B293" t="s">
         <v>9</v>
@@ -9254,7 +9254,7 @@
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B294" t="s">
         <v>9</v>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B295" t="s">
         <v>9</v>
@@ -9300,7 +9300,7 @@
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B296" t="s">
         <v>9</v>
@@ -9323,7 +9323,7 @@
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B297" t="s">
         <v>9</v>
@@ -9346,7 +9346,7 @@
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B298" t="s">
         <v>9</v>
@@ -9369,7 +9369,7 @@
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B299" t="s">
         <v>9</v>
@@ -9392,7 +9392,7 @@
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B300" t="s">
         <v>9</v>
@@ -9415,7 +9415,7 @@
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B301" t="s">
         <v>9</v>
@@ -9438,7 +9438,7 @@
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B302" t="s">
         <v>9</v>
@@ -9461,7 +9461,7 @@
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B303" t="s">
         <v>9</v>
@@ -9490,7 +9490,7 @@
     </row>
     <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B304" t="s">
         <v>9</v>
@@ -9508,12 +9508,12 @@
         <v>38220</v>
       </c>
       <c r="G304" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B305" t="s">
         <v>9</v>
@@ -9542,7 +9542,7 @@
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B306" t="s">
         <v>9</v>
@@ -9565,7 +9565,7 @@
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B307" t="s">
         <v>9</v>
@@ -9588,7 +9588,7 @@
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B308" t="s">
         <v>9</v>
@@ -9611,7 +9611,7 @@
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B309" t="s">
         <v>9</v>
@@ -9634,7 +9634,7 @@
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B310" t="s">
         <v>9</v>
@@ -9657,7 +9657,7 @@
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B311" t="s">
         <v>9</v>
@@ -9680,7 +9680,7 @@
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B312" t="s">
         <v>9</v>
@@ -9703,7 +9703,7 @@
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B313" t="s">
         <v>9</v>
@@ -9726,7 +9726,7 @@
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B314" t="s">
         <v>9</v>
@@ -9749,7 +9749,7 @@
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B315" t="s">
         <v>9</v>
@@ -9772,7 +9772,7 @@
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B316" t="s">
         <v>9</v>
@@ -9795,7 +9795,7 @@
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B317" t="s">
         <v>9</v>
@@ -9818,7 +9818,7 @@
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B318" t="s">
         <v>9</v>
@@ -9847,7 +9847,7 @@
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B319" t="s">
         <v>9</v>
@@ -9870,7 +9870,7 @@
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B320" t="s">
         <v>9</v>
@@ -9893,7 +9893,7 @@
     </row>
     <row r="321" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B321" t="s">
         <v>9</v>
@@ -9920,12 +9920,12 @@
         <v>12</v>
       </c>
       <c r="P321" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="322" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B322" t="s">
         <v>9</v>
@@ -9954,7 +9954,7 @@
     </row>
     <row r="323" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B323" t="s">
         <v>9</v>
@@ -9977,7 +9977,7 @@
     </row>
     <row r="324" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B324" t="s">
         <v>9</v>
@@ -10000,7 +10000,7 @@
     </row>
     <row r="325" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B325" t="s">
         <v>9</v>
@@ -10023,7 +10023,7 @@
     </row>
     <row r="326" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B326" t="s">
         <v>9</v>
@@ -10046,7 +10046,7 @@
     </row>
     <row r="327" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B327" t="s">
         <v>9</v>
@@ -10064,12 +10064,12 @@
         <v>38293</v>
       </c>
       <c r="G327" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="328" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B328" t="s">
         <v>9</v>
@@ -10087,12 +10087,12 @@
         <v>38295</v>
       </c>
       <c r="G328" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="329" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B329" t="s">
         <v>9</v>
@@ -10115,7 +10115,7 @@
     </row>
     <row r="330" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B330" t="s">
         <v>9</v>
@@ -10138,7 +10138,7 @@
     </row>
     <row r="331" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B331" t="s">
         <v>9</v>
@@ -10161,7 +10161,7 @@
     </row>
     <row r="332" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B332" t="s">
         <v>9</v>
@@ -10184,7 +10184,7 @@
     </row>
     <row r="333" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B333" t="s">
         <v>9</v>
@@ -10213,7 +10213,7 @@
     </row>
     <row r="334" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B334" t="s">
         <v>9</v>
@@ -10236,7 +10236,7 @@
     </row>
     <row r="335" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B335" t="s">
         <v>9</v>
@@ -10259,7 +10259,7 @@
     </row>
     <row r="336" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B336" t="s">
         <v>9</v>
@@ -10282,7 +10282,7 @@
     </row>
     <row r="337" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B337" t="s">
         <v>9</v>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="338" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B338" t="s">
         <v>9</v>
@@ -10328,7 +10328,7 @@
     </row>
     <row r="339" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B339" t="s">
         <v>9</v>
@@ -10346,7 +10346,7 @@
         <v>38314</v>
       </c>
       <c r="G339" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H339" t="s">
         <v>10</v>
@@ -10357,7 +10357,7 @@
     </row>
     <row r="340" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B340" t="s">
         <v>9</v>
@@ -10380,7 +10380,7 @@
     </row>
     <row r="341" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B341" t="s">
         <v>9</v>
@@ -10403,7 +10403,7 @@
     </row>
     <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B342" t="s">
         <v>9</v>
@@ -10426,7 +10426,7 @@
     </row>
     <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B343" t="s">
         <v>9</v>
@@ -10449,7 +10449,7 @@
     </row>
     <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B344" t="s">
         <v>9</v>
@@ -10472,7 +10472,7 @@
     </row>
     <row r="345" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B345" t="s">
         <v>9</v>
@@ -10495,7 +10495,7 @@
     </row>
     <row r="346" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B346" t="s">
         <v>9</v>
@@ -10518,7 +10518,7 @@
     </row>
     <row r="347" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B347" t="s">
         <v>9</v>
@@ -10541,7 +10541,7 @@
     </row>
     <row r="348" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B348" t="s">
         <v>9</v>
@@ -10562,12 +10562,12 @@
         <v>52</v>
       </c>
       <c r="P348" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="349" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B349" t="s">
         <v>9</v>
@@ -10590,7 +10590,7 @@
     </row>
     <row r="350" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B350" t="s">
         <v>9</v>
@@ -10613,7 +10613,7 @@
     </row>
     <row r="351" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B351" t="s">
         <v>9</v>
@@ -10636,7 +10636,7 @@
     </row>
     <row r="352" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B352" t="s">
         <v>9</v>
@@ -10657,12 +10657,12 @@
         <v>52</v>
       </c>
       <c r="P352" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="353" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B353" t="s">
         <v>9</v>
@@ -10685,7 +10685,7 @@
     </row>
     <row r="354" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B354" t="s">
         <v>9</v>
@@ -10708,7 +10708,7 @@
     </row>
     <row r="355" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B355" t="s">
         <v>9</v>
@@ -10731,7 +10731,7 @@
     </row>
     <row r="356" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B356" t="s">
         <v>9</v>
@@ -10754,7 +10754,7 @@
     </row>
     <row r="357" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B357" t="s">
         <v>9</v>
@@ -10777,7 +10777,7 @@
     </row>
     <row r="358" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B358" t="s">
         <v>9</v>
@@ -10800,7 +10800,7 @@
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B359" t="s">
         <v>9</v>
@@ -10823,7 +10823,7 @@
     </row>
     <row r="360" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B360" t="s">
         <v>9</v>
@@ -10846,7 +10846,7 @@
     </row>
     <row r="361" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B361" t="s">
         <v>9</v>
@@ -10869,7 +10869,7 @@
     </row>
     <row r="362" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B362" t="s">
         <v>9</v>
@@ -10892,7 +10892,7 @@
     </row>
     <row r="363" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B363" t="s">
         <v>9</v>
@@ -10915,7 +10915,7 @@
     </row>
     <row r="364" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B364" t="s">
         <v>9</v>
@@ -10938,7 +10938,7 @@
     </row>
     <row r="365" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B365" t="s">
         <v>9</v>
@@ -10961,7 +10961,7 @@
     </row>
     <row r="366" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B366" t="s">
         <v>9</v>
@@ -10984,7 +10984,7 @@
     </row>
     <row r="367" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B367" t="s">
         <v>9</v>
@@ -11007,7 +11007,7 @@
     </row>
     <row r="368" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B368" t="s">
         <v>9</v>
@@ -11034,12 +11034,12 @@
         <v>12</v>
       </c>
       <c r="P368" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B369" t="s">
         <v>9</v>
@@ -11068,7 +11068,7 @@
     </row>
     <row r="370" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B370" t="s">
         <v>9</v>
@@ -11091,7 +11091,7 @@
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B371" t="s">
         <v>9</v>
@@ -11114,7 +11114,7 @@
     </row>
     <row r="372" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B372" t="s">
         <v>9</v>
@@ -11137,7 +11137,7 @@
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B373" t="s">
         <v>9</v>
@@ -11160,7 +11160,7 @@
     </row>
     <row r="374" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B374" t="s">
         <v>9</v>
@@ -11183,7 +11183,7 @@
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B375" t="s">
         <v>9</v>
@@ -11206,7 +11206,7 @@
     </row>
     <row r="376" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B376" t="s">
         <v>9</v>
@@ -11229,7 +11229,7 @@
     </row>
     <row r="377" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B377" t="s">
         <v>9</v>
@@ -11252,7 +11252,7 @@
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B378" t="s">
         <v>9</v>
@@ -11275,7 +11275,7 @@
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B379" t="s">
         <v>9</v>
@@ -11298,7 +11298,7 @@
     </row>
     <row r="380" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B380" t="s">
         <v>9</v>
@@ -11321,7 +11321,7 @@
     </row>
     <row r="381" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B381" t="s">
         <v>9</v>
@@ -11344,7 +11344,7 @@
     </row>
     <row r="382" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B382" t="s">
         <v>9</v>
@@ -11367,7 +11367,7 @@
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B383" t="s">
         <v>9</v>
@@ -11390,7 +11390,7 @@
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B384" t="s">
         <v>9</v>
@@ -11413,7 +11413,7 @@
     </row>
     <row r="385" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B385" t="s">
         <v>9</v>
@@ -11440,12 +11440,12 @@
         <v>12</v>
       </c>
       <c r="P385" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="386" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B386" t="s">
         <v>9</v>
@@ -11474,7 +11474,7 @@
     </row>
     <row r="387" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B387" t="s">
         <v>9</v>
@@ -11497,7 +11497,7 @@
     </row>
     <row r="388" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B388" t="s">
         <v>9</v>
@@ -11520,7 +11520,7 @@
     </row>
     <row r="389" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B389" t="s">
         <v>9</v>
@@ -11541,12 +11541,12 @@
         <v>52</v>
       </c>
       <c r="P389" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="390" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B390" t="s">
         <v>9</v>
@@ -11569,7 +11569,7 @@
     </row>
     <row r="391" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B391" t="s">
         <v>9</v>
@@ -11592,7 +11592,7 @@
     </row>
     <row r="392" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B392" t="s">
         <v>9</v>
@@ -11615,7 +11615,7 @@
     </row>
     <row r="393" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B393" t="s">
         <v>9</v>
@@ -11638,7 +11638,7 @@
     </row>
     <row r="394" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B394" t="s">
         <v>9</v>
@@ -11661,7 +11661,7 @@
     </row>
     <row r="395" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B395" t="s">
         <v>9</v>
@@ -11684,7 +11684,7 @@
     </row>
     <row r="396" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B396" t="s">
         <v>9</v>
@@ -11707,7 +11707,7 @@
     </row>
     <row r="397" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B397" t="s">
         <v>9</v>
@@ -11730,7 +11730,7 @@
     </row>
     <row r="398" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B398" t="s">
         <v>9</v>
@@ -11753,7 +11753,7 @@
     </row>
     <row r="399" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B399" t="s">
         <v>9</v>
@@ -11776,7 +11776,7 @@
     </row>
     <row r="400" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B400" t="s">
         <v>9</v>
@@ -11799,7 +11799,7 @@
     </row>
     <row r="401" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B401" t="s">
         <v>9</v>
@@ -11822,7 +11822,7 @@
     </row>
     <row r="402" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B402" t="s">
         <v>9</v>
@@ -11845,7 +11845,7 @@
     </row>
     <row r="403" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B403" t="s">
         <v>9</v>
@@ -11868,7 +11868,7 @@
     </row>
     <row r="404" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B404" t="s">
         <v>9</v>
@@ -11891,7 +11891,7 @@
     </row>
     <row r="405" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B405" t="s">
         <v>9</v>
@@ -11914,7 +11914,7 @@
     </row>
     <row r="406" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B406" t="s">
         <v>9</v>
@@ -11937,7 +11937,7 @@
     </row>
     <row r="407" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B407" t="s">
         <v>9</v>
@@ -11960,7 +11960,7 @@
     </row>
     <row r="408" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B408" t="s">
         <v>9</v>
@@ -11983,7 +11983,7 @@
     </row>
     <row r="409" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B409" t="s">
         <v>9</v>
@@ -12006,7 +12006,7 @@
     </row>
     <row r="410" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B410" t="s">
         <v>9</v>
@@ -12029,7 +12029,7 @@
     </row>
     <row r="411" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B411" t="s">
         <v>9</v>
@@ -12052,7 +12052,7 @@
     </row>
     <row r="412" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B412" t="s">
         <v>9</v>
@@ -12075,7 +12075,7 @@
     </row>
     <row r="413" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B413" t="s">
         <v>9</v>
@@ -12098,7 +12098,7 @@
     </row>
     <row r="414" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B414" t="s">
         <v>9</v>
@@ -12125,12 +12125,12 @@
         <v>12</v>
       </c>
       <c r="P414" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="415" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B415" t="s">
         <v>9</v>
@@ -12159,7 +12159,7 @@
     </row>
     <row r="416" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B416" t="s">
         <v>9</v>
@@ -12182,7 +12182,7 @@
     </row>
     <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B417" t="s">
         <v>9</v>
@@ -12200,12 +12200,12 @@
         <v>38659</v>
       </c>
       <c r="G417" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B418" t="s">
         <v>9</v>
@@ -12228,7 +12228,7 @@
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B419" t="s">
         <v>9</v>
@@ -12257,7 +12257,7 @@
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B420" t="s">
         <v>9</v>
@@ -12280,7 +12280,7 @@
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B421" t="s">
         <v>9</v>
@@ -12298,7 +12298,7 @@
         <v>38664</v>
       </c>
       <c r="G421" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H421" t="s">
         <v>10</v>
@@ -12309,7 +12309,7 @@
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B422" t="s">
         <v>9</v>
@@ -12338,7 +12338,7 @@
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B423" t="s">
         <v>9</v>
@@ -12361,7 +12361,7 @@
     </row>
     <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B424" t="s">
         <v>9</v>
@@ -12384,7 +12384,7 @@
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B425" t="s">
         <v>9</v>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B426" t="s">
         <v>9</v>
@@ -12433,7 +12433,7 @@
     </row>
     <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B427" t="s">
         <v>9</v>
@@ -12456,7 +12456,7 @@
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B428" t="s">
         <v>9</v>
@@ -12479,7 +12479,7 @@
     </row>
     <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B429" t="s">
         <v>9</v>
@@ -12502,7 +12502,7 @@
     </row>
     <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B430" t="s">
         <v>9</v>
@@ -12525,7 +12525,7 @@
     </row>
     <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B431" t="s">
         <v>9</v>
@@ -12548,7 +12548,7 @@
     </row>
     <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B432" t="s">
         <v>9</v>
@@ -12571,7 +12571,7 @@
     </row>
     <row r="433" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B433" t="s">
         <v>9</v>
@@ -12594,7 +12594,7 @@
     </row>
     <row r="434" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B434" t="s">
         <v>9</v>
@@ -12617,7 +12617,7 @@
     </row>
     <row r="435" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B435" t="s">
         <v>9</v>
@@ -12640,7 +12640,7 @@
     </row>
     <row r="436" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B436" t="s">
         <v>9</v>
@@ -12663,7 +12663,7 @@
     </row>
     <row r="437" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B437" t="s">
         <v>9</v>
@@ -12686,7 +12686,7 @@
     </row>
     <row r="438" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B438" t="s">
         <v>9</v>
@@ -12704,12 +12704,12 @@
         <v>38685</v>
       </c>
       <c r="G438" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="439" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B439" t="s">
         <v>9</v>
@@ -12738,7 +12738,7 @@
     </row>
     <row r="440" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B440" t="s">
         <v>9</v>
@@ -12761,7 +12761,7 @@
     </row>
     <row r="441" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B441" t="s">
         <v>9</v>
@@ -12790,7 +12790,7 @@
     </row>
     <row r="442" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B442" t="s">
         <v>9</v>
@@ -12813,7 +12813,7 @@
     </row>
     <row r="443" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B443" t="s">
         <v>9</v>
@@ -12836,7 +12836,7 @@
     </row>
     <row r="444" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B444" t="s">
         <v>9</v>
@@ -12863,12 +12863,12 @@
         <v>12</v>
       </c>
       <c r="P444" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="445" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B445" t="s">
         <v>9</v>
@@ -12897,7 +12897,7 @@
     </row>
     <row r="446" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B446" t="s">
         <v>9</v>
@@ -12920,7 +12920,7 @@
     </row>
     <row r="447" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B447" t="s">
         <v>9</v>
@@ -12943,7 +12943,7 @@
     </row>
     <row r="448" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B448" t="s">
         <v>9</v>
@@ -12961,12 +12961,12 @@
         <v>38783</v>
       </c>
       <c r="G448" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="449" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B449" t="s">
         <v>9</v>
@@ -12989,7 +12989,7 @@
     </row>
     <row r="450" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B450" t="s">
         <v>9</v>
@@ -13012,7 +13012,7 @@
     </row>
     <row r="451" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B451" t="s">
         <v>9</v>
@@ -13035,7 +13035,7 @@
     </row>
     <row r="452" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B452" t="s">
         <v>9</v>
@@ -13065,12 +13065,12 @@
         <v>10</v>
       </c>
       <c r="P452" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="453" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B453" t="s">
         <v>9</v>
@@ -13099,7 +13099,7 @@
     </row>
     <row r="454" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B454" t="s">
         <v>9</v>
@@ -13122,7 +13122,7 @@
     </row>
     <row r="455" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B455" t="s">
         <v>9</v>
@@ -13145,7 +13145,7 @@
     </row>
     <row r="456" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B456" t="s">
         <v>9</v>
@@ -13168,7 +13168,7 @@
     </row>
     <row r="457" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B457" t="s">
         <v>9</v>
@@ -13191,7 +13191,7 @@
     </row>
     <row r="458" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B458" t="s">
         <v>9</v>
@@ -13214,7 +13214,7 @@
     </row>
     <row r="459" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B459" t="s">
         <v>9</v>
@@ -13237,7 +13237,7 @@
     </row>
     <row r="460" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B460" t="s">
         <v>9</v>
@@ -13260,7 +13260,7 @@
     </row>
     <row r="461" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B461" t="s">
         <v>9</v>
@@ -13289,7 +13289,7 @@
     </row>
     <row r="462" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B462" t="s">
         <v>9</v>
@@ -13321,7 +13321,7 @@
     </row>
     <row r="463" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B463" t="s">
         <v>9</v>
@@ -13350,7 +13350,7 @@
     </row>
     <row r="464" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B464" t="s">
         <v>9</v>
@@ -13373,7 +13373,7 @@
     </row>
     <row r="465" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B465" t="s">
         <v>9</v>
@@ -13396,7 +13396,7 @@
     </row>
     <row r="466" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B466" t="s">
         <v>9</v>
@@ -13419,7 +13419,7 @@
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B467" t="s">
         <v>9</v>
@@ -13442,7 +13442,7 @@
     </row>
     <row r="468" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B468" t="s">
         <v>9</v>
@@ -13460,12 +13460,12 @@
         <v>38922</v>
       </c>
       <c r="G468" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="469" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B469" t="s">
         <v>9</v>
@@ -13488,7 +13488,7 @@
     </row>
     <row r="470" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B470" t="s">
         <v>9</v>
@@ -13511,7 +13511,7 @@
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B471" t="s">
         <v>9</v>
@@ -13540,7 +13540,7 @@
     </row>
     <row r="472" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B472" t="s">
         <v>9</v>
@@ -13558,12 +13558,12 @@
         <v>38985</v>
       </c>
       <c r="G472" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B473" t="s">
         <v>9</v>
@@ -13586,7 +13586,7 @@
     </row>
     <row r="474" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B474" t="s">
         <v>9</v>
@@ -13609,7 +13609,7 @@
     </row>
     <row r="475" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B475" t="s">
         <v>9</v>
@@ -13632,7 +13632,7 @@
     </row>
     <row r="476" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B476" t="s">
         <v>9</v>
@@ -13655,7 +13655,7 @@
     </row>
     <row r="477" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B477" t="s">
         <v>9</v>
@@ -13673,12 +13673,12 @@
         <v>39014</v>
       </c>
       <c r="G477" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="478" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B478" t="s">
         <v>9</v>
@@ -13701,7 +13701,7 @@
     </row>
     <row r="479" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B479" t="s">
         <v>9</v>
@@ -13724,7 +13724,7 @@
     </row>
     <row r="480" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B480" t="s">
         <v>9</v>
@@ -13747,7 +13747,7 @@
     </row>
     <row r="481" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B481" t="s">
         <v>9</v>
@@ -13770,7 +13770,7 @@
     </row>
     <row r="482" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B482" t="s">
         <v>9</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="483" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B483" t="s">
         <v>9</v>
@@ -13811,12 +13811,12 @@
         <v>39035</v>
       </c>
       <c r="G483" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="484" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B484" t="s">
         <v>9</v>
@@ -13834,12 +13834,12 @@
         <v>39035</v>
       </c>
       <c r="G484" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="485" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B485" t="s">
         <v>9</v>
@@ -13862,7 +13862,7 @@
     </row>
     <row r="486" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B486" t="s">
         <v>9</v>
@@ -13885,7 +13885,7 @@
     </row>
     <row r="487" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B487" t="s">
         <v>9</v>
@@ -13908,7 +13908,7 @@
     </row>
     <row r="488" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B488" t="s">
         <v>9</v>
@@ -13931,7 +13931,7 @@
     </row>
     <row r="489" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B489" t="s">
         <v>9</v>
@@ -13954,7 +13954,7 @@
     </row>
     <row r="490" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B490" t="s">
         <v>9</v>
@@ -13983,7 +13983,7 @@
     </row>
     <row r="491" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B491" t="s">
         <v>9</v>
@@ -14006,7 +14006,7 @@
     </row>
     <row r="492" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B492" t="s">
         <v>9</v>
@@ -14024,12 +14024,12 @@
         <v>39170</v>
       </c>
       <c r="G492" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="493" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B493" t="s">
         <v>9</v>
@@ -14047,12 +14047,12 @@
         <v>39234</v>
       </c>
       <c r="G493" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="494" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B494" t="s">
         <v>9</v>
@@ -14081,7 +14081,7 @@
     </row>
     <row r="495" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B495" t="s">
         <v>28</v>
@@ -14108,7 +14108,7 @@
         <v>10</v>
       </c>
       <c r="P495" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="496" spans="1:16" x14ac:dyDescent="0.25">
@@ -16181,7 +16181,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added css placeholders and site update
</commit_message>
<xml_diff>
--- a/collection.xlsx
+++ b/collection.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4772" uniqueCount="1499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="1691">
   <si>
     <t>Platform</t>
   </si>
@@ -4515,6 +4515,582 @@
   </si>
   <si>
     <t>Lord of the Rings The Two Towers</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aG5zxXX.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IwhKBNT.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/q6MidXx.jpg</t>
+  </si>
+  <si>
+    <t>The Elder Scrolls 3: Morrowind</t>
+  </si>
+  <si>
+    <t>Serious Sam 2</t>
+  </si>
+  <si>
+    <t>Broken Sword The Sleeping Dragon</t>
+  </si>
+  <si>
+    <t>Oddworld Strangers Wrath</t>
+  </si>
+  <si>
+    <t>Conker Live &amp; Reloaded</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zoWKlH7.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aIeaxSV.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8Xfx6L5.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/i5Wv6gB.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/kLqqRBD.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/gyc2JFC.jpg</t>
+  </si>
+  <si>
+    <t>Tribal</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GFbqB9r.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NnCLBcj.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/VWCUC3k.jpg</t>
+  </si>
+  <si>
+    <t>Resident Evil The Umbrella Chronicles</t>
+  </si>
+  <si>
+    <t>Dokapon Kingdom</t>
+  </si>
+  <si>
+    <t>25th anniversary edition</t>
+  </si>
+  <si>
+    <t>Zelda Skyward Sword</t>
+  </si>
+  <si>
+    <t>Trauma Center New Blood</t>
+  </si>
+  <si>
+    <t>Het Studio 100 Speeleiland</t>
+  </si>
+  <si>
+    <t>Samurai Shodown Anthology</t>
+  </si>
+  <si>
+    <t>Major Minor's Majestic March</t>
+  </si>
+  <si>
+    <t>Kid Paddle Lost in the Game</t>
+  </si>
+  <si>
+    <t>Chaos A La Maison</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/g428CPw.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9KXHKMi.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/YTUcIkM.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/UbViEHN.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/EQHLkI5.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IOorswg.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/UAPTFPV.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ulscsxc.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/mfOHa6T.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oygOOte.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oW5QAAC.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/opdNDMj.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/uZ78Kf0.jpg</t>
+  </si>
+  <si>
+    <t>Ninety-Nine Nights</t>
+  </si>
+  <si>
+    <t>Ninja Gaiden 2</t>
+  </si>
+  <si>
+    <t>Lost Odyssey</t>
+  </si>
+  <si>
+    <t>Shadowrun</t>
+  </si>
+  <si>
+    <t>Duke Nukem Forever</t>
+  </si>
+  <si>
+    <t>Dark Messiah of Might and Magic Elements</t>
+  </si>
+  <si>
+    <t>Enslaved Odyssey to the West</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>World of Tanks</t>
+  </si>
+  <si>
+    <t>Beautiful Katamari</t>
+  </si>
+  <si>
+    <t>Kameo Elements of Power</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NKeEYfq.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/We4tt2F.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xfQHC0p.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/SVAq4JH.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IvsBZDF.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/VQ3R0gA.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Vdp1pdn.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/jdyg74s.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/av1JQcv.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/YNtYVX7.jpg</t>
+  </si>
+  <si>
+    <t>LOTR: The Battle for Middle-Earth 2</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/3npqdkK.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/hHeohcz.jpg</t>
+  </si>
+  <si>
+    <t>Ni No Kuni 2 Revenant Kingdom</t>
+  </si>
+  <si>
+    <t>King's Edition</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/g7bxRog.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/FsJH49I.jpg</t>
+  </si>
+  <si>
+    <t>Pokemon Ultra Moon</t>
+  </si>
+  <si>
+    <t>Pokemon Ultra Sun</t>
+  </si>
+  <si>
+    <t>Fan Edition</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/D47EwBJ.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/CnbVNeR.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/H0A8wqw.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ec151V0.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aZXmLxn.jpg</t>
+  </si>
+  <si>
+    <t>Modern Colours Mario</t>
+  </si>
+  <si>
+    <t>Dragon Age Origins</t>
+  </si>
+  <si>
+    <t>Bioshock 2</t>
+  </si>
+  <si>
+    <t>Rapture Edition</t>
+  </si>
+  <si>
+    <t>Ratchet &amp; Clank Trilogy</t>
+  </si>
+  <si>
+    <t>Dead Rising 2</t>
+  </si>
+  <si>
+    <t>Metal Gear Rising Revengeance</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z Budokai HD Collection</t>
+  </si>
+  <si>
+    <t>Dragon Age 2</t>
+  </si>
+  <si>
+    <t>NeverDead</t>
+  </si>
+  <si>
+    <t>Lollipop Chainsaw</t>
+  </si>
+  <si>
+    <t>Motorstorm</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z Burst Limit</t>
+  </si>
+  <si>
+    <t>Singularity</t>
+  </si>
+  <si>
+    <t>Call of Duty Ghosts</t>
+  </si>
+  <si>
+    <t>Untold Legends Dark Kingdom</t>
+  </si>
+  <si>
+    <t>Medal of Honor</t>
+  </si>
+  <si>
+    <t>Everybody's Golf World Tour</t>
+  </si>
+  <si>
+    <t>Tomb Raider</t>
+  </si>
+  <si>
+    <t>Final Fantasy XIII</t>
+  </si>
+  <si>
+    <t>Silent Hill HD Collection</t>
+  </si>
+  <si>
+    <t>Sports Champions</t>
+  </si>
+  <si>
+    <t>Resistance Fall Of Man</t>
+  </si>
+  <si>
+    <t>Skate 3</t>
+  </si>
+  <si>
+    <t>Red Dead Redemption</t>
+  </si>
+  <si>
+    <t>Operation Flashpoint Dragon Rising</t>
+  </si>
+  <si>
+    <t>F1 Championship Edition</t>
+  </si>
+  <si>
+    <t>Playstation Move Starter Disc</t>
+  </si>
+  <si>
+    <t>Midway Arcade Origins</t>
+  </si>
+  <si>
+    <t>Journey</t>
+  </si>
+  <si>
+    <t>Wipeout HD Fury</t>
+  </si>
+  <si>
+    <t>Vampire Rain Altered Species</t>
+  </si>
+  <si>
+    <t>Siren Blood Curse</t>
+  </si>
+  <si>
+    <t>The House of the Dead Overkill</t>
+  </si>
+  <si>
+    <t>Lord of the Rings Conquest</t>
+  </si>
+  <si>
+    <t>Fairytale Fights</t>
+  </si>
+  <si>
+    <t>Beyond Two Souls</t>
+  </si>
+  <si>
+    <t>The Last Of Us</t>
+  </si>
+  <si>
+    <t>Dishonored</t>
+  </si>
+  <si>
+    <t>GOTY</t>
+  </si>
+  <si>
+    <t>Resident Evil 5</t>
+  </si>
+  <si>
+    <t>Steelbook</t>
+  </si>
+  <si>
+    <t>Valkyria Chronicles</t>
+  </si>
+  <si>
+    <t>Castlevania Lords of Shadow</t>
+  </si>
+  <si>
+    <t>Castlevania Lords of Shadow 2</t>
+  </si>
+  <si>
+    <t>Brutal Legend</t>
+  </si>
+  <si>
+    <t>Tekken Hybrid</t>
+  </si>
+  <si>
+    <t>Devil May Cry HD Collection</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts HD 1.5 Remix</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts HD 2.5 Remix</t>
+  </si>
+  <si>
+    <t>Zone of the Enders HD Collection</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto 5</t>
+  </si>
+  <si>
+    <t>God Of War Collection</t>
+  </si>
+  <si>
+    <t>The Club</t>
+  </si>
+  <si>
+    <t>Tales of Xillia 2</t>
+  </si>
+  <si>
+    <t>Day One Edition</t>
+  </si>
+  <si>
+    <t>Tales of Symphonia Chronicles</t>
+  </si>
+  <si>
+    <t>Call of Duty 4 Modern Warfare</t>
+  </si>
+  <si>
+    <t>Fallout 3</t>
+  </si>
+  <si>
+    <t>Viking Battle for Asgard</t>
+  </si>
+  <si>
+    <t>Splinter Cell Trilogy</t>
+  </si>
+  <si>
+    <t>Mega Drive Ultimate Collection</t>
+  </si>
+  <si>
+    <t>Ratchet &amp; Clank A Crack in Time</t>
+  </si>
+  <si>
+    <t>Ratchet &amp; Clank Quest for Booty</t>
+  </si>
+  <si>
+    <t>Ratchet &amp; Clank Tools of Destruction</t>
+  </si>
+  <si>
+    <t>God of War 3</t>
+  </si>
+  <si>
+    <t>The ICO &amp; Shadow of the Colossus Collection</t>
+  </si>
+  <si>
+    <t>Ni No Kuni Wrath of the White Witch</t>
+  </si>
+  <si>
+    <t>Folklore</t>
+  </si>
+  <si>
+    <t>God of War Collection Volume 2</t>
+  </si>
+  <si>
+    <t>Modnotion Racers</t>
+  </si>
+  <si>
+    <t>Heavy Rain</t>
+  </si>
+  <si>
+    <t>LittleBigPlanet</t>
+  </si>
+  <si>
+    <t>Prince of Persia Trilogy</t>
+  </si>
+  <si>
+    <t>Ar Nosurge Ode to an Unborn Star</t>
+  </si>
+  <si>
+    <t>Uncharted Drake's Fortune</t>
+  </si>
+  <si>
+    <t>Uncharted 2 Among Thieves</t>
+  </si>
+  <si>
+    <t>Uncharted 3 Drake's Deception</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QlbqZwh.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/siBqzoO.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/vUxqDSk.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9q8hA5b.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WcJgOea.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IKQtOcZ.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NrG3Irt.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TjWRNe4.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Zs34Pdg.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DMDI8xq.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/58m4bWx.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/os6TttE.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/2lXUTbe.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/FIKmnzP.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/jxsoalT.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WZDboEl.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XKZGLo8.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/7jkqfKz.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/1HKbxAV.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/O5LwXJR.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/hEny3Bo.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/YBmgwtS.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/gyxeUsm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/yFaRGbp.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8nV8eJA.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/wu81m6e.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/AZtJc7q.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/yaTNTSU.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/BOwUCCL.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/hT7mWF5.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DlyOpMG.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/w9b5wmN.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zdbXdE9.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TLJ9Lwv.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9c2sn7z.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/deNCLTQ.jpg</t>
   </si>
 </sst>
 </file>
@@ -4885,11 +5461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N956"/>
+  <dimension ref="A1:N1065"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A995" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1016" sqref="A1016"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6296,6 +6872,9 @@
       <c r="H59" t="s">
         <v>9</v>
       </c>
+      <c r="J59" t="s">
+        <v>1516</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -14869,6 +15448,9 @@
       <c r="E534" t="s">
         <v>46</v>
       </c>
+      <c r="J534" t="s">
+        <v>1501</v>
+      </c>
     </row>
     <row r="535" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
@@ -14886,6 +15468,9 @@
       <c r="E535" t="s">
         <v>46</v>
       </c>
+      <c r="J535" t="s">
+        <v>1499</v>
+      </c>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A536" s="2" t="s">
@@ -14903,6 +15488,9 @@
       <c r="E536" t="s">
         <v>46</v>
       </c>
+      <c r="J536" t="s">
+        <v>1500</v>
+      </c>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
@@ -15265,6 +15853,9 @@
       <c r="E555" t="s">
         <v>46</v>
       </c>
+      <c r="J555" t="s">
+        <v>1512</v>
+      </c>
     </row>
     <row r="556" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A556" s="5" t="s">
@@ -23692,6 +24283,1874 @@
       </c>
       <c r="J956" t="s">
         <v>1492</v>
+      </c>
+    </row>
+    <row r="957" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A957" s="2" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B957" t="s">
+        <v>28</v>
+      </c>
+      <c r="C957" t="s">
+        <v>600</v>
+      </c>
+      <c r="E957" t="s">
+        <v>46</v>
+      </c>
+      <c r="J957" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="958" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A958" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B958" t="s">
+        <v>28</v>
+      </c>
+      <c r="C958" t="s">
+        <v>600</v>
+      </c>
+      <c r="E958" t="s">
+        <v>46</v>
+      </c>
+      <c r="J958" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="959" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A959" s="2" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B959" t="s">
+        <v>28</v>
+      </c>
+      <c r="C959" t="s">
+        <v>600</v>
+      </c>
+      <c r="E959" t="s">
+        <v>46</v>
+      </c>
+      <c r="J959" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="960" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A960" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B960" t="s">
+        <v>28</v>
+      </c>
+      <c r="C960" t="s">
+        <v>600</v>
+      </c>
+      <c r="E960" t="s">
+        <v>46</v>
+      </c>
+      <c r="J960" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="961" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A961" s="2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B961" t="s">
+        <v>28</v>
+      </c>
+      <c r="C961" t="s">
+        <v>600</v>
+      </c>
+      <c r="E961" t="s">
+        <v>46</v>
+      </c>
+      <c r="J961" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="962" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A962" s="2" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B962" t="s">
+        <v>13</v>
+      </c>
+      <c r="C962" t="s">
+        <v>602</v>
+      </c>
+      <c r="D962" s="1">
+        <v>37064</v>
+      </c>
+      <c r="E962" t="s">
+        <v>46</v>
+      </c>
+      <c r="F962" t="s">
+        <v>1513</v>
+      </c>
+      <c r="J962" t="s">
+        <v>1514</v>
+      </c>
+      <c r="K962" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="963" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A963" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B963" t="s">
+        <v>22</v>
+      </c>
+      <c r="C963" t="s">
+        <v>601</v>
+      </c>
+      <c r="E963" t="s">
+        <v>46</v>
+      </c>
+      <c r="J963" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="964" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A964" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B964" t="s">
+        <v>22</v>
+      </c>
+      <c r="C964" t="s">
+        <v>600</v>
+      </c>
+      <c r="E964" t="s">
+        <v>46</v>
+      </c>
+      <c r="J964" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="965" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A965" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B965" t="s">
+        <v>22</v>
+      </c>
+      <c r="C965" t="s">
+        <v>600</v>
+      </c>
+      <c r="E965" t="s">
+        <v>46</v>
+      </c>
+      <c r="F965" t="s">
+        <v>1519</v>
+      </c>
+      <c r="J965" t="s">
+        <v>1529</v>
+      </c>
+      <c r="K965" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="966" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A966" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B966" t="s">
+        <v>22</v>
+      </c>
+      <c r="C966" t="s">
+        <v>600</v>
+      </c>
+      <c r="E966" t="s">
+        <v>46</v>
+      </c>
+      <c r="F966" t="s">
+        <v>605</v>
+      </c>
+      <c r="J966" t="s">
+        <v>1531</v>
+      </c>
+      <c r="K966" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="967" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A967" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B967" t="s">
+        <v>22</v>
+      </c>
+      <c r="C967" t="s">
+        <v>600</v>
+      </c>
+      <c r="E967" t="s">
+        <v>46</v>
+      </c>
+      <c r="J967" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="968" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A968" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B968" t="s">
+        <v>22</v>
+      </c>
+      <c r="C968" t="s">
+        <v>600</v>
+      </c>
+      <c r="E968" t="s">
+        <v>46</v>
+      </c>
+      <c r="J968" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="969" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A969" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B969" t="s">
+        <v>22</v>
+      </c>
+      <c r="C969" t="s">
+        <v>18</v>
+      </c>
+      <c r="E969" t="s">
+        <v>46</v>
+      </c>
+      <c r="J969" t="s">
+        <v>1535</v>
+      </c>
+      <c r="K969" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="970" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A970" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B970" t="s">
+        <v>22</v>
+      </c>
+      <c r="C970" t="s">
+        <v>18</v>
+      </c>
+      <c r="E970" t="s">
+        <v>46</v>
+      </c>
+      <c r="J970" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="971" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A971" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B971" t="s">
+        <v>22</v>
+      </c>
+      <c r="C971" t="s">
+        <v>600</v>
+      </c>
+      <c r="E971" t="s">
+        <v>46</v>
+      </c>
+      <c r="J971" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="972" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A972" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B972" t="s">
+        <v>22</v>
+      </c>
+      <c r="C972" t="s">
+        <v>600</v>
+      </c>
+      <c r="E972" t="s">
+        <v>46</v>
+      </c>
+      <c r="J972" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="973" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A973" s="2" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B973" t="s">
+        <v>29</v>
+      </c>
+      <c r="C973" t="s">
+        <v>600</v>
+      </c>
+      <c r="E973" t="s">
+        <v>46</v>
+      </c>
+      <c r="J973" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="974" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A974" s="2" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B974" t="s">
+        <v>29</v>
+      </c>
+      <c r="C974" t="s">
+        <v>600</v>
+      </c>
+      <c r="E974" t="s">
+        <v>46</v>
+      </c>
+      <c r="J974" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="975" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A975" s="2" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B975" t="s">
+        <v>29</v>
+      </c>
+      <c r="C975" t="s">
+        <v>600</v>
+      </c>
+      <c r="E975" t="s">
+        <v>46</v>
+      </c>
+      <c r="J975" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="976" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A976" s="2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B976" t="s">
+        <v>29</v>
+      </c>
+      <c r="C976" t="s">
+        <v>600</v>
+      </c>
+      <c r="E976" t="s">
+        <v>46</v>
+      </c>
+      <c r="J976" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="977" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A977" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B977" t="s">
+        <v>29</v>
+      </c>
+      <c r="C977" t="s">
+        <v>600</v>
+      </c>
+      <c r="E977" t="s">
+        <v>46</v>
+      </c>
+      <c r="J977" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="978" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A978" s="2" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B978" t="s">
+        <v>29</v>
+      </c>
+      <c r="C978" t="s">
+        <v>600</v>
+      </c>
+      <c r="E978" t="s">
+        <v>46</v>
+      </c>
+      <c r="J978" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="979" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A979" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B979" t="s">
+        <v>29</v>
+      </c>
+      <c r="C979" t="s">
+        <v>600</v>
+      </c>
+      <c r="E979" t="s">
+        <v>46</v>
+      </c>
+      <c r="J979" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="980" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A980" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B980" t="s">
+        <v>29</v>
+      </c>
+      <c r="C980" t="s">
+        <v>600</v>
+      </c>
+      <c r="E980" t="s">
+        <v>46</v>
+      </c>
+      <c r="J980" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="981" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A981" s="2" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B981" t="s">
+        <v>29</v>
+      </c>
+      <c r="C981" t="s">
+        <v>600</v>
+      </c>
+      <c r="E981" t="s">
+        <v>46</v>
+      </c>
+      <c r="J981" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="982" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A982" s="2" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B982" t="s">
+        <v>29</v>
+      </c>
+      <c r="C982" t="s">
+        <v>600</v>
+      </c>
+      <c r="E982" t="s">
+        <v>46</v>
+      </c>
+      <c r="J982" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="983" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A983" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B983" t="s">
+        <v>29</v>
+      </c>
+      <c r="C983" t="s">
+        <v>600</v>
+      </c>
+      <c r="E983" t="s">
+        <v>46</v>
+      </c>
+      <c r="J983" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="984" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A984" s="2" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B984" t="s">
+        <v>29</v>
+      </c>
+      <c r="C984" t="s">
+        <v>600</v>
+      </c>
+      <c r="E984" t="s">
+        <v>46</v>
+      </c>
+      <c r="J984" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="985" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A985" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B985" t="s">
+        <v>27</v>
+      </c>
+      <c r="C985" t="s">
+        <v>18</v>
+      </c>
+      <c r="E985" t="s">
+        <v>46</v>
+      </c>
+      <c r="J985" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="986" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A986" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B986" t="s">
+        <v>27</v>
+      </c>
+      <c r="C986" t="s">
+        <v>18</v>
+      </c>
+      <c r="E986" t="s">
+        <v>46</v>
+      </c>
+      <c r="F986" t="s">
+        <v>1565</v>
+      </c>
+      <c r="J986" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="987" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A987" s="2" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B987" t="s">
+        <v>34</v>
+      </c>
+      <c r="C987" t="s">
+        <v>600</v>
+      </c>
+      <c r="E987" t="s">
+        <v>46</v>
+      </c>
+      <c r="F987" t="s">
+        <v>1570</v>
+      </c>
+      <c r="J987" t="s">
+        <v>1571</v>
+      </c>
+      <c r="K987" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="988" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A988" s="2" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B988" t="s">
+        <v>34</v>
+      </c>
+      <c r="C988" t="s">
+        <v>18</v>
+      </c>
+      <c r="E988" t="s">
+        <v>46</v>
+      </c>
+      <c r="F988" t="s">
+        <v>1570</v>
+      </c>
+      <c r="J988" t="s">
+        <v>1573</v>
+      </c>
+      <c r="K988" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="989" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A989" s="2" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B989" t="s">
+        <v>11</v>
+      </c>
+      <c r="C989" t="s">
+        <v>18</v>
+      </c>
+      <c r="J989" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="990" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A990" s="2" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B990" t="s">
+        <v>26</v>
+      </c>
+      <c r="C990" t="s">
+        <v>600</v>
+      </c>
+      <c r="E990" t="s">
+        <v>46</v>
+      </c>
+      <c r="J990" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="991" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A991" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B991" t="s">
+        <v>26</v>
+      </c>
+      <c r="C991" t="s">
+        <v>600</v>
+      </c>
+      <c r="E991" t="s">
+        <v>46</v>
+      </c>
+      <c r="F991" t="s">
+        <v>1579</v>
+      </c>
+      <c r="J991" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="992" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A992" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B992" t="s">
+        <v>26</v>
+      </c>
+      <c r="C992" t="s">
+        <v>600</v>
+      </c>
+      <c r="E992" t="s">
+        <v>46</v>
+      </c>
+      <c r="J992" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="993" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A993" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B993" t="s">
+        <v>26</v>
+      </c>
+      <c r="C993" t="s">
+        <v>600</v>
+      </c>
+      <c r="E993" t="s">
+        <v>46</v>
+      </c>
+      <c r="G993" t="s">
+        <v>7</v>
+      </c>
+      <c r="J993" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="994" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A994" s="2" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B994" t="s">
+        <v>26</v>
+      </c>
+      <c r="C994" t="s">
+        <v>18</v>
+      </c>
+      <c r="E994" t="s">
+        <v>46</v>
+      </c>
+      <c r="J994" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="995" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A995" s="2" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B995" t="s">
+        <v>26</v>
+      </c>
+      <c r="C995" t="s">
+        <v>18</v>
+      </c>
+      <c r="E995" t="s">
+        <v>46</v>
+      </c>
+      <c r="J995" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="996" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A996" s="2" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B996" t="s">
+        <v>26</v>
+      </c>
+      <c r="C996" t="s">
+        <v>600</v>
+      </c>
+      <c r="E996" t="s">
+        <v>46</v>
+      </c>
+      <c r="J996" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="997" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A997" s="2" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B997" t="s">
+        <v>26</v>
+      </c>
+      <c r="C997" t="s">
+        <v>600</v>
+      </c>
+      <c r="E997" t="s">
+        <v>46</v>
+      </c>
+      <c r="J997" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="998" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A998" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B998" t="s">
+        <v>26</v>
+      </c>
+      <c r="C998" t="s">
+        <v>18</v>
+      </c>
+      <c r="E998" t="s">
+        <v>46</v>
+      </c>
+      <c r="J998" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="999" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A999" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B999" t="s">
+        <v>26</v>
+      </c>
+      <c r="C999" t="s">
+        <v>18</v>
+      </c>
+      <c r="E999" t="s">
+        <v>46</v>
+      </c>
+      <c r="J999" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1000" s="2" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1000" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1001" s="2" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1001" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1002" s="2" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1002" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1003" s="2" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1003" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1003" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1004" s="2" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1004" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1005" s="2" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1005" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1006" s="2" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1006" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1007" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1007" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1008" s="2" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1008" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1008" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1008" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1009" s="2" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1009" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1010" s="2" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1010" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1011" s="2" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1011" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1012" s="2" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1012" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1013" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1013" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1014" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1014" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1014" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1014" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1015" s="2" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1015" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1016" s="2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1016" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1017" s="2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>601</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1017" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1018" s="2" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1018" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1019" s="2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>660</v>
+      </c>
+      <c r="G1019" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1019" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1019" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1020" s="2" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1020" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1021" s="2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1021" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1022" s="2" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1022" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1023" s="2" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1023" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1024" s="2" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1024" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1024" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1025" s="2" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1025" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1025" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1025" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1026" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1027" s="2" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1027" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1027" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1028" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1028" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1029" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1029" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1030" s="2" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1031" s="2" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1032" s="2" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>601</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1033" s="2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1033" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1033" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1034" s="2" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1035" s="2" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1036" s="2" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1037" s="2" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1038" s="2" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1039" s="2" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1040" s="2" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1041" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1042" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1043" s="2" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1044" s="2" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1045" s="2" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1046" s="2" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1047" s="2" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1047" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1048" s="2" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1049" s="2" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1050" s="2" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1051" s="2" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1052" s="2" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1053" s="2" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1054" s="2" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G1054" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1054" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1055" s="2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1055" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1055" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1056" s="2" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1057" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1058" s="2" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1058" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1058" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1059" s="2" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1060" s="2" t="s">
+        <v>1649</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1060" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1060" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1061" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1062" s="2" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1063" s="2" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1063" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1063" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1064" s="2" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1064" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1064" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1065" s="2" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>600</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -23702,7 +26161,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Platforms!$A:$A</xm:f>

</xml_diff>